<commit_message>
VOC was taken off from the BOM
</commit_message>
<xml_diff>
--- a/Project Flow Documents/Project Documents/BOM.xlsx
+++ b/Project Flow Documents/Project Documents/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
   <si>
     <t>Part #</t>
   </si>
@@ -93,21 +93,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>VOC sensor for air-quality monitor</t>
-  </si>
-  <si>
-    <t>http://www.aliexpress.com/item/5pcs-lot-FIGARO-air-quality-VOC-gas-sensor-TGS2602/1956331481.html</t>
-  </si>
-  <si>
-    <t>China(Mainland)</t>
-  </si>
-  <si>
-    <t>AliExpress</t>
-  </si>
-  <si>
-    <t>VOC Sensor</t>
-  </si>
-  <si>
     <t>Accelerometer</t>
   </si>
   <si>
@@ -291,16 +276,10 @@
     <t>TC33X-2-104E</t>
   </si>
   <si>
-    <t>TGS2602*</t>
-  </si>
-  <si>
     <t>P4SMA7.5CA-E3/5A**</t>
   </si>
   <si>
-    <t>** Cell H12 indicates the price for 100 units.</t>
-  </si>
-  <si>
-    <t>*A quotation has been requested from Figaro.</t>
+    <t>* Cell H12 indicates the price for 100 units.</t>
   </si>
 </sst>
 </file>
@@ -372,7 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -391,9 +370,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -701,9 +677,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -747,186 +723,187 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="F2" s="9">
         <v>5</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="H2" s="11">
-        <v>5.95</v>
+        <v>7.55</v>
       </c>
       <c r="I2" s="11">
-        <v>29.72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="9">
+        <f t="shared" ref="I2:I16" si="0">F2*H2</f>
+        <v>37.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43.15" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2">
         <v>5</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" s="11">
-        <v>7.55</v>
-      </c>
-      <c r="I3" s="11">
-        <f t="shared" ref="I3:I17" si="0">F3*H3</f>
-        <v>37.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="43.15" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="H3" s="5">
+        <v>9.01</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" si="0"/>
+        <v>45.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F4" s="2">
         <v>5</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H4" s="5">
-        <v>9.01</v>
+        <v>1.27</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" si="0"/>
-        <v>45.05</v>
+        <v>6.35</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F5" s="2">
         <v>5</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H5" s="5">
-        <v>1.27</v>
+        <v>1.08</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="0"/>
-        <v>6.35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="3" t="s">
         <v>35</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F6" s="2">
         <v>5</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H6" s="5">
-        <v>1.08</v>
+        <v>0.97</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="0"/>
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>4.8499999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="F7" s="2">
         <v>5</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H7" s="5">
-        <v>0.97</v>
+        <v>0.91</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="0"/>
-        <v>4.8499999999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -934,162 +911,162 @@
         <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="2">
-        <v>5</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="H8" s="5">
-        <v>0.91</v>
+        <v>1.46</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="0"/>
-        <v>4.55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F9" s="2">
         <v>5</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H9" s="5">
-        <v>1.46</v>
+        <v>3.95</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="0"/>
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+        <v>19.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="F10" s="2">
         <v>5</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H10" s="5">
-        <v>3.95</v>
+        <v>0.89</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="0"/>
-        <v>19.75</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F11" s="2">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>55</v>
       </c>
       <c r="H11" s="5">
-        <v>0.89</v>
+        <v>0.219</v>
       </c>
       <c r="I11" s="5">
+        <v>0.219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="I12" s="5">
         <f t="shared" si="0"/>
-        <v>4.45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.9" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="2">
-        <v>100</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0.219</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0.219</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>67</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F13" s="2">
         <v>5</v>
@@ -1098,28 +1075,28 @@
         <v>64</v>
       </c>
       <c r="H13" s="5">
-        <v>0.6</v>
+        <v>0.75275999999999998</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>3.7637999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="F14" s="2">
         <v>5</v>
@@ -1128,11 +1105,11 @@
         <v>69</v>
       </c>
       <c r="H14" s="5">
-        <v>0.75275999999999998</v>
+        <v>1.33</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="0"/>
-        <v>3.7637999999999998</v>
+        <v>6.65</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
@@ -1140,181 +1117,143 @@
         <v>75</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>76</v>
       </c>
       <c r="F15" s="2">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H15" s="5">
-        <v>1.33</v>
+        <v>0.35</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="0"/>
-        <v>6.65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="F16" s="2">
-        <v>15</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="H16" s="5">
-        <v>0.35</v>
+        <v>0.27</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="0"/>
-        <v>5.25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>88</v>
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="2">
+        <v>5</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="6">
+        <v>15</v>
+      </c>
+      <c r="I17" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="8">
+        <f>SUM(H2:H17)</f>
+        <v>45.611760000000004</v>
+      </c>
+      <c r="I18" s="5">
+        <f>SUM(I2:I17)</f>
+        <v>235.68279999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="2">
-        <v>5</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0.27</v>
-      </c>
-      <c r="I17" s="5">
-        <f t="shared" si="0"/>
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="2">
-        <v>5</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="6">
-        <v>15</v>
-      </c>
-      <c r="I18" s="6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="8">
-        <f>SUM(H2:H18)</f>
-        <v>51.561760000000007</v>
-      </c>
-      <c r="I19" s="5">
-        <f>SUM(I2:I18)</f>
-        <v>265.40280000000001</v>
-      </c>
+      <c r="B20" s="14"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="14"/>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" s="15"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G24" s="1"/>
+      <c r="G22" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
+  <mergeCells count="2">
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A20:B20"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1"/>
-    <hyperlink ref="G5" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3" display="http://www.mouser.com/hiroseconnector/"/>
-    <hyperlink ref="G2" r:id="rId4"/>
-    <hyperlink ref="C8" r:id="rId5" display="http://digikey.com/Suppliers/us/Semtech.page?lang=en"/>
+    <hyperlink ref="G3" r:id="rId1"/>
+    <hyperlink ref="G4" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3" display="http://www.mouser.com/hiroseconnector/"/>
+    <hyperlink ref="C7" r:id="rId4" display="http://digikey.com/Suppliers/us/Semtech.page?lang=en"/>
+    <hyperlink ref="G9" r:id="rId5"/>
     <hyperlink ref="G10" r:id="rId6"/>
-    <hyperlink ref="G11" r:id="rId7"/>
-    <hyperlink ref="G8" r:id="rId8"/>
-    <hyperlink ref="C12" r:id="rId9" display="http://www.mouser.com/vishaysemiconductors/"/>
-    <hyperlink ref="C13" r:id="rId10" display="http://digikey.com/Suppliers/us/Fairchild-Semiconductor.page?lang=en"/>
-    <hyperlink ref="C14" r:id="rId11" display="http://digikey.com/Suppliers/us/Elna-America.page?lang=en"/>
-    <hyperlink ref="C15" r:id="rId12" display="http://digikey.com/Suppliers/us/C-and-K-Components.page?lang=en"/>
-    <hyperlink ref="C3" r:id="rId13" display="http://digikey.com/Suppliers/us/Analog-Devices.page?lang=en"/>
-    <hyperlink ref="G17" r:id="rId14"/>
-    <hyperlink ref="G16" r:id="rId15"/>
-    <hyperlink ref="G12" r:id="rId16"/>
+    <hyperlink ref="G7" r:id="rId7"/>
+    <hyperlink ref="C11" r:id="rId8" display="http://www.mouser.com/vishaysemiconductors/"/>
+    <hyperlink ref="C12" r:id="rId9" display="http://digikey.com/Suppliers/us/Fairchild-Semiconductor.page?lang=en"/>
+    <hyperlink ref="C13" r:id="rId10" display="http://digikey.com/Suppliers/us/Elna-America.page?lang=en"/>
+    <hyperlink ref="C14" r:id="rId11" display="http://digikey.com/Suppliers/us/C-and-K-Components.page?lang=en"/>
+    <hyperlink ref="C2" r:id="rId12" display="http://digikey.com/Suppliers/us/Analog-Devices.page?lang=en"/>
+    <hyperlink ref="G16" r:id="rId13"/>
+    <hyperlink ref="G15" r:id="rId14"/>
+    <hyperlink ref="G11" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>